<commit_message>
Add LoadingScene and Thread
</commit_message>
<xml_diff>
--- a/ErrorSolution.xlsx
+++ b/ErrorSolution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93b8cf70261917fc/바탕 화면/Dx12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{F3492A7B-C779-43AE-A478-E93FA17D9E4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A00E6C96-F22C-4B83-81B9-906F5A77A266}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{F3492A7B-C779-43AE-A478-E93FA17D9E4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E713583C-C2F4-43E8-B54E-57E6D6135956}"/>
   <bookViews>
-    <workbookView xWindow="-25500" yWindow="2115" windowWidth="21600" windowHeight="12165" xr2:uid="{814D8898-1336-43D0-933C-AD0290055E40}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{814D8898-1336-43D0-933C-AD0290055E40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>오류 코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -125,6 +125,14 @@
   </si>
   <si>
     <t>상수버퍼였는데, 쉐이더 리소스 뷰 셋을 해버림</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Textures created with certain Formats must align the resource dimensions properly. D3D12_RESOURCE_DESC::Format is BC3_UNORM. D3D12_RESOURCE_DESC::Width is 512, and must be a multiple of 4. D3D12_RESOURCE_DESC::Height is 170, and must be a multiple of 4. [ STATE_CREATION ERROR #597: CREATERESOURCE_INVALIDDIMENSIONS]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밉맵추출을 위해 dds는 4의 배수 텍스쳐야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,9 +533,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{491BA09D-4026-4342-A1C9-7A84BE33E748}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -637,6 +645,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="15" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>